<commit_message>
200107 creditplus wijmo 연습
</commit_message>
<xml_diff>
--- a/creditplus_copy/문서/DB.xlsx
+++ b/creditplus_copy/문서/DB.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="93">
   <si>
     <t>고객번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -245,10 +245,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>model</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>accid</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -354,6 +350,50 @@
   </si>
   <si>
     <t>외감 대기업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>modeldiv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>업력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COM_HISTORY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>순서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hisno</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hiscontent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hisdate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COM_HISTORY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>accgroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>계정그룹</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -771,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:X26"/>
+  <dimension ref="B1:X34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -823,7 +863,7 @@
         <v>41</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q3" s="8"/>
     </row>
@@ -866,7 +906,7 @@
         <v>1</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.3">
@@ -903,7 +943,7 @@
         <v>2</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.3">
@@ -939,10 +979,20 @@
         <v>3</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B7" s="3">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="3"/>
       <c r="G7" s="3">
         <v>3</v>
       </c>
@@ -950,7 +1000,7 @@
         <v>53</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>47</v>
@@ -967,10 +1017,10 @@
         <v>4</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>47</v>
@@ -993,7 +1043,7 @@
         <v>54</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>47</v>
@@ -1005,7 +1055,7 @@
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="P9" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q9" s="10"/>
       <c r="X9" t="s">
@@ -1013,11 +1063,29 @@
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="G10" s="3">
+        <v>6</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
       <c r="P10" s="3">
         <v>1</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X10" t="s">
         <v>6</v>
@@ -1028,103 +1096,85 @@
         <v>2</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="G12" t="s">
-        <v>43</v>
-      </c>
       <c r="P12" s="3">
         <v>3</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="X12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="G13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>30</v>
+      <c r="G13" t="s">
+        <v>43</v>
       </c>
       <c r="P13" s="6">
         <v>4</v>
       </c>
       <c r="Q13" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="X13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="G14" s="3">
-        <v>1</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="K14" s="3">
-        <v>10</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
+      <c r="G14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="X14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.3">
       <c r="G15" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>47</v>
       </c>
       <c r="K15" s="3">
+        <v>10</v>
+      </c>
+      <c r="L15" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="X15" t="s">
@@ -1132,8 +1182,26 @@
       </c>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="G16" s="3">
+        <v>2</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K16" s="3">
+        <v>45</v>
+      </c>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
       <c r="P16" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q16" s="10"/>
       <c r="X16" t="s">
@@ -1141,126 +1209,102 @@
       </c>
     </row>
     <row r="17" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G17" s="3">
+        <v>2</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K17" s="3">
+        <v>3</v>
+      </c>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
       <c r="P17" s="3">
         <v>1</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="X17" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="7:24" x14ac:dyDescent="0.3">
-      <c r="G18" t="s">
-        <v>42</v>
-      </c>
       <c r="P18" s="3">
         <v>2</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="X18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="7:24" x14ac:dyDescent="0.3">
-      <c r="G19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="P19" s="3">
         <v>3</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="X19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="7:24" x14ac:dyDescent="0.3">
-      <c r="G20" s="3">
-        <v>1</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="K20" s="3">
-        <v>10</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
+      <c r="G20" t="s">
+        <v>42</v>
+      </c>
       <c r="X20" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="7:24" x14ac:dyDescent="0.3">
-      <c r="G21" s="3">
-        <v>2</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="K21" s="3">
-        <v>10</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="M21" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="N21" s="3"/>
+      <c r="G21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="X21" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G22" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>47</v>
@@ -1271,12 +1315,10 @@
       <c r="L22" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="M22" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="M22" s="3"/>
       <c r="N22" s="3"/>
       <c r="P22" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q22" s="10"/>
       <c r="X22" t="s">
@@ -1285,28 +1327,32 @@
     </row>
     <row r="23" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G23" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K23" s="3">
-        <v>18</v>
-      </c>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="M23" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="N23" s="3"/>
       <c r="P23" s="3">
         <v>1</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="X23" t="s">
         <v>18</v>
@@ -1314,28 +1360,32 @@
     </row>
     <row r="24" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G24" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K24" s="3">
-        <v>9</v>
-      </c>
-      <c r="L24" s="5"/>
-      <c r="M24" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="N24" s="3"/>
       <c r="P24" s="3">
         <v>2</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X24" t="s">
         <v>23</v>
@@ -1343,19 +1393,19 @@
     </row>
     <row r="25" spans="7:24" x14ac:dyDescent="0.3">
       <c r="G25" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K25" s="3">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
@@ -1364,16 +1414,151 @@
         <v>3</v>
       </c>
       <c r="Q25" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="X25" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="26" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G26" s="3">
+        <v>5</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K26" s="3">
+        <v>9</v>
+      </c>
+      <c r="L26" s="5"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
       <c r="X26" t="s">
         <v>22</v>
       </c>
+    </row>
+    <row r="29" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G29" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G31" s="3">
+        <v>1</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="M31" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="N31" s="3"/>
+    </row>
+    <row r="32" spans="7:24" x14ac:dyDescent="0.3">
+      <c r="G32" s="3">
+        <v>2</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K32" s="3">
+        <v>10</v>
+      </c>
+      <c r="L32" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="M32" s="5"/>
+      <c r="N32" s="3"/>
+    </row>
+    <row r="33" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G33" s="3">
+        <v>3</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K33" s="3">
+        <v>300</v>
+      </c>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="3"/>
+    </row>
+    <row r="34" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G34" s="3">
+        <v>4</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K34" s="3">
+        <v>9</v>
+      </c>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>